<commit_message>
Added the optee work under Raspbain screen.
</commit_message>
<xml_diff>
--- a/doc/SingtelIOTProjectPlan.xlsx
+++ b/doc/SingtelIOTProjectPlan.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>About This Template</t>
   </si>
@@ -155,9 +155,6 @@
     <t xml:space="preserve">Database management  part + user authorization </t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>Jun Wen Wong, Mohamed Haroon Basheer and  LiuYuancheng</t>
@@ -191,28 +185,10 @@
     <t xml:space="preserve">Assigned </t>
   </si>
   <si>
-    <t>Design improvement and fixed the detial module need to implement</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attestation with the gateway [25 June] </t>
   </si>
   <si>
     <t>Use Trust Zone to protect the gateway program</t>
-  </si>
-  <si>
-    <t>GateWay full disk encryption and protection.</t>
-  </si>
-  <si>
-    <t>GateWay full disk encryption [ 14 July]</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
   </si>
   <si>
     <t xml:space="preserve">Problem analysis  + Define scope + System design </t>
@@ -234,6 +210,15 @@
   </si>
   <si>
     <t>July</t>
+  </si>
+  <si>
+    <t>Design improvement and fixed the detail module need to implement</t>
+  </si>
+  <si>
+    <t>Gateway full disk encryption [ 14 July]</t>
+  </si>
+  <si>
+    <t>Gateway full disk encryption and protection.</t>
   </si>
 </sst>
 </file>
@@ -900,24 +885,6 @@
     <xf numFmtId="37" fontId="0" fillId="10" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyBorder="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="5" borderId="3" xfId="9" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="5" borderId="4" xfId="9" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -963,6 +930,24 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="5" borderId="3" xfId="9" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="5" borderId="4" xfId="9" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Bad" xfId="13" builtinId="27"/>
@@ -983,6 +968,30 @@
     <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1128,30 +1137,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1410,7 +1395,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>219074</xdr:colOff>
+          <xdr:colOff>219075</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -1462,7 +1447,7 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Milestone Description" dataDxfId="8"/>
+    <tableColumn id="1" name="Milestone Description" dataDxfId="0"/>
     <tableColumn id="3" name="Assigned "/>
     <tableColumn id="4" name="Progress"/>
     <tableColumn id="5" name="Start"/>
@@ -1746,7 +1731,7 @@
   <dimension ref="A1:BZ30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BM5" sqref="BM5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1755,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1"/>
@@ -1785,14 +1770,14 @@
       <c r="B2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64">
+      <c r="D2" s="80"/>
+      <c r="E2" s="81">
         <v>43556</v>
       </c>
-      <c r="F2" s="65"/>
+      <c r="F2" s="82"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
@@ -1804,13 +1789,13 @@
       <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="62" t="s">
+      <c r="B3" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="63"/>
+      <c r="D3" s="80"/>
       <c r="E3" s="36">
         <v>0</v>
       </c>
@@ -1825,10 +1810,10 @@
       <c r="A4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="67"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="37">
         <v>3</v>
       </c>
@@ -1920,7 +1905,7 @@
       <c r="BM4" s="17"/>
       <c r="BN4" s="17"/>
       <c r="BO4" s="17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="BP4" s="17"/>
       <c r="BQ4" s="17"/>
@@ -1928,7 +1913,7 @@
       <c r="BS4" s="17"/>
       <c r="BT4" s="17"/>
       <c r="BU4" s="17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="BV4" s="17"/>
       <c r="BW4" s="17"/>
@@ -2196,7 +2181,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>4</v>
@@ -2438,10 +2423,10 @@
       <c r="BO6" s="44"/>
       <c r="BP6" s="44"/>
       <c r="BQ6" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="BR6" s="44" t="s">
         <v>33</v>
-      </c>
-      <c r="BR6" s="44" t="s">
-        <v>34</v>
       </c>
       <c r="BS6" s="44"/>
       <c r="BT6" s="44"/>
@@ -2450,11 +2435,11 @@
       <c r="BW6" s="44"/>
       <c r="BX6" s="44"/>
       <c r="BY6" s="44"/>
-      <c r="BZ6" s="84" t="s">
-        <v>32</v>
+      <c r="BZ6" s="78" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:78" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
@@ -2525,8 +2510,8 @@
       <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="78" t="s">
-        <v>52</v>
+      <c r="B8" s="72" t="s">
+        <v>44</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="50"/>
@@ -2813,24 +2798,24 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E8,$F8=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ8" s="75" t="str">
+      <c r="BZ8" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E8,$F8=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="69"/>
+      <c r="B9" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="63"/>
       <c r="D9" s="24">
         <v>1</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="64">
         <v>43556</v>
       </c>
-      <c r="F9" s="71"/>
+      <c r="F9" s="65"/>
       <c r="G9" s="20"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
@@ -2874,40 +2859,40 @@
       <c r="AU9" s="56"/>
       <c r="AV9" s="56"/>
       <c r="AW9" s="56"/>
-      <c r="AX9" s="72"/>
-      <c r="AY9" s="72"/>
-      <c r="AZ9" s="72"/>
-      <c r="BA9" s="72"/>
-      <c r="BB9" s="72"/>
-      <c r="BC9" s="72"/>
-      <c r="BD9" s="72"/>
-      <c r="BE9" s="72"/>
-      <c r="BF9" s="72"/>
-      <c r="BG9" s="72"/>
-      <c r="BH9" s="72"/>
-      <c r="BI9" s="72"/>
-      <c r="BJ9" s="72"/>
-      <c r="BK9" s="72"/>
-      <c r="BL9" s="72"/>
-      <c r="BM9" s="72"/>
-      <c r="BN9" s="72"/>
-      <c r="BO9" s="72"/>
-      <c r="BP9" s="72"/>
-      <c r="BQ9" s="72"/>
-      <c r="BR9" s="72"/>
-      <c r="BS9" s="72"/>
-      <c r="BT9" s="72"/>
-      <c r="BU9" s="72"/>
-      <c r="BV9" s="72"/>
-      <c r="BW9" s="72"/>
-      <c r="BX9" s="72"/>
-      <c r="BY9" s="72"/>
-      <c r="BZ9" s="72"/>
+      <c r="AX9" s="66"/>
+      <c r="AY9" s="66"/>
+      <c r="AZ9" s="66"/>
+      <c r="BA9" s="66"/>
+      <c r="BB9" s="66"/>
+      <c r="BC9" s="66"/>
+      <c r="BD9" s="66"/>
+      <c r="BE9" s="66"/>
+      <c r="BF9" s="66"/>
+      <c r="BG9" s="66"/>
+      <c r="BH9" s="66"/>
+      <c r="BI9" s="66"/>
+      <c r="BJ9" s="66"/>
+      <c r="BK9" s="66"/>
+      <c r="BL9" s="66"/>
+      <c r="BM9" s="66"/>
+      <c r="BN9" s="66"/>
+      <c r="BO9" s="66"/>
+      <c r="BP9" s="66"/>
+      <c r="BQ9" s="66"/>
+      <c r="BR9" s="66"/>
+      <c r="BS9" s="66"/>
+      <c r="BT9" s="66"/>
+      <c r="BU9" s="66"/>
+      <c r="BV9" s="66"/>
+      <c r="BW9" s="66"/>
+      <c r="BX9" s="66"/>
+      <c r="BY9" s="66"/>
+      <c r="BZ9" s="66"/>
     </row>
     <row r="10" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="73" t="s">
-        <v>39</v>
+      <c r="B10" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="24">
@@ -3188,14 +3173,14 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E11,$F11=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ10" s="75" t="str">
+      <c r="BZ10" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E11,$F11=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="67" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="27"/>
@@ -3479,15 +3464,15 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E12,$F12=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ11" s="75" t="str">
+      <c r="BZ11" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E12,$F12=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="73" t="s">
-        <v>40</v>
+      <c r="B12" s="67" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="24">
@@ -3509,7 +3494,7 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
-      <c r="N12" s="75" t="str">
+      <c r="N12" s="69" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(N$5=$E12,$F12=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -3753,15 +3738,15 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ12" s="75" t="str">
+      <c r="BZ12" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="73" t="s">
-        <v>41</v>
+      <c r="B13" s="67" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="24">
@@ -3790,11 +3775,11 @@
         <f ca="1">IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(K$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="L13" s="75" t="str">
+      <c r="L13" s="69" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(L$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="M13" s="75" t="str">
+      <c r="M13" s="69" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(M$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -3802,11 +3787,11 @@
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
-      <c r="R13" s="75" t="str">
+      <c r="R13" s="69" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(R$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="S13" s="75" t="str">
+      <c r="S13" s="69" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(S$5=$E13,$F13=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -4030,14 +4015,14 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=#REF!,#REF!=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ13" s="75" t="str">
+      <c r="BZ13" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=#REF!,#REF!=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="68" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="27"/>
@@ -4322,15 +4307,15 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E16,$F16=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ14" s="75" t="str">
+      <c r="BZ14" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E16,$F16=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="73" t="s">
-        <v>43</v>
+      <c r="B15" s="67" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="24">
@@ -4368,7 +4353,7 @@
       <c r="AD15" s="19"/>
       <c r="AE15" s="19"/>
       <c r="AF15" s="19"/>
-      <c r="AG15" s="75"/>
+      <c r="AG15" s="69"/>
       <c r="AH15" s="28"/>
       <c r="AI15" s="28"/>
       <c r="AJ15" s="28"/>
@@ -4413,12 +4398,12 @@
       <c r="BW15" s="28"/>
       <c r="BX15" s="28"/>
       <c r="BY15" s="28"/>
-      <c r="BZ15" s="75"/>
+      <c r="BZ15" s="69"/>
     </row>
     <row r="16" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="79" t="s">
-        <v>38</v>
+      <c r="B16" s="73" t="s">
+        <v>36</v>
       </c>
       <c r="C16" s="58"/>
       <c r="D16" s="59"/>
@@ -4705,7 +4690,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E17,$F17=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ16" s="75" t="str">
+      <c r="BZ16" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E17,$F17=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -4973,7 +4958,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E18,$F18=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ17" s="75" t="str">
+      <c r="BZ17" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E18,$F18=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -5247,7 +5232,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E19,$F19=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ18" s="75" t="str">
+      <c r="BZ18" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E19,$F19=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -5533,7 +5518,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E20,$F20=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ19" s="75" t="str">
+      <c r="BZ19" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E20,$F20=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -5828,7 +5813,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E21,$F21=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ20" s="75" t="str">
+      <c r="BZ20" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E21,$F21=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -5836,7 +5821,7 @@
     <row r="21" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="24">
@@ -6117,7 +6102,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E22,$F22=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ21" s="75" t="str">
+      <c r="BZ21" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E22,$F22=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -6125,7 +6110,7 @@
     <row r="22" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="29" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="24">
@@ -6415,7 +6400,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E23,$F23=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ22" s="75" t="str">
+      <c r="BZ22" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E23,$F23=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -6423,7 +6408,7 @@
     <row r="23" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="24">
@@ -6701,7 +6686,7 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E25,$F25=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ23" s="75" t="str">
+      <c r="BZ23" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E25,$F25=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -6710,90 +6695,90 @@
       <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="80" t="s">
-        <v>44</v>
+      <c r="B24" s="74" t="s">
+        <v>41</v>
       </c>
       <c r="C24" s="58"/>
       <c r="D24" s="59"/>
       <c r="E24" s="60"/>
       <c r="F24" s="61"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="77"/>
-      <c r="S24" s="77"/>
-      <c r="T24" s="77"/>
-      <c r="U24" s="77"/>
-      <c r="V24" s="77"/>
-      <c r="W24" s="77"/>
-      <c r="X24" s="77"/>
-      <c r="Y24" s="77"/>
-      <c r="Z24" s="77"/>
-      <c r="AA24" s="77"/>
-      <c r="AB24" s="77"/>
-      <c r="AC24" s="77"/>
-      <c r="AD24" s="77"/>
-      <c r="AE24" s="77"/>
-      <c r="AF24" s="77"/>
-      <c r="AG24" s="77"/>
-      <c r="AH24" s="77"/>
-      <c r="AI24" s="77"/>
-      <c r="AJ24" s="77"/>
-      <c r="AK24" s="77"/>
-      <c r="AL24" s="77"/>
-      <c r="AM24" s="77"/>
-      <c r="AN24" s="77"/>
-      <c r="AO24" s="77"/>
-      <c r="AP24" s="77"/>
-      <c r="AQ24" s="77"/>
-      <c r="AR24" s="77"/>
-      <c r="AS24" s="77"/>
-      <c r="AT24" s="77"/>
-      <c r="AU24" s="77"/>
-      <c r="AV24" s="77"/>
-      <c r="AW24" s="77"/>
-      <c r="AX24" s="77"/>
-      <c r="AY24" s="77"/>
-      <c r="AZ24" s="77"/>
-      <c r="BA24" s="77"/>
-      <c r="BB24" s="77"/>
-      <c r="BC24" s="77"/>
-      <c r="BD24" s="77"/>
-      <c r="BE24" s="77"/>
-      <c r="BF24" s="77"/>
-      <c r="BG24" s="77"/>
-      <c r="BH24" s="77"/>
-      <c r="BI24" s="77"/>
-      <c r="BJ24" s="77"/>
-      <c r="BK24" s="77"/>
-      <c r="BL24" s="77"/>
-      <c r="BM24" s="77"/>
-      <c r="BN24" s="77"/>
-      <c r="BO24" s="77"/>
-      <c r="BP24" s="77"/>
-      <c r="BQ24" s="77"/>
-      <c r="BR24" s="77"/>
-      <c r="BS24" s="77"/>
-      <c r="BT24" s="77"/>
-      <c r="BU24" s="77"/>
-      <c r="BV24" s="77"/>
-      <c r="BW24" s="77"/>
-      <c r="BX24" s="77"/>
-      <c r="BY24" s="77"/>
-      <c r="BZ24" s="77"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="71"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="71"/>
+      <c r="U24" s="71"/>
+      <c r="V24" s="71"/>
+      <c r="W24" s="71"/>
+      <c r="X24" s="71"/>
+      <c r="Y24" s="71"/>
+      <c r="Z24" s="71"/>
+      <c r="AA24" s="71"/>
+      <c r="AB24" s="71"/>
+      <c r="AC24" s="71"/>
+      <c r="AD24" s="71"/>
+      <c r="AE24" s="71"/>
+      <c r="AF24" s="71"/>
+      <c r="AG24" s="71"/>
+      <c r="AH24" s="71"/>
+      <c r="AI24" s="71"/>
+      <c r="AJ24" s="71"/>
+      <c r="AK24" s="71"/>
+      <c r="AL24" s="71"/>
+      <c r="AM24" s="71"/>
+      <c r="AN24" s="71"/>
+      <c r="AO24" s="71"/>
+      <c r="AP24" s="71"/>
+      <c r="AQ24" s="71"/>
+      <c r="AR24" s="71"/>
+      <c r="AS24" s="71"/>
+      <c r="AT24" s="71"/>
+      <c r="AU24" s="71"/>
+      <c r="AV24" s="71"/>
+      <c r="AW24" s="71"/>
+      <c r="AX24" s="71"/>
+      <c r="AY24" s="71"/>
+      <c r="AZ24" s="71"/>
+      <c r="BA24" s="71"/>
+      <c r="BB24" s="71"/>
+      <c r="BC24" s="71"/>
+      <c r="BD24" s="71"/>
+      <c r="BE24" s="71"/>
+      <c r="BF24" s="71"/>
+      <c r="BG24" s="71"/>
+      <c r="BH24" s="71"/>
+      <c r="BI24" s="71"/>
+      <c r="BJ24" s="71"/>
+      <c r="BK24" s="71"/>
+      <c r="BL24" s="71"/>
+      <c r="BM24" s="71"/>
+      <c r="BN24" s="71"/>
+      <c r="BO24" s="71"/>
+      <c r="BP24" s="71"/>
+      <c r="BQ24" s="71"/>
+      <c r="BR24" s="71"/>
+      <c r="BS24" s="71"/>
+      <c r="BT24" s="71"/>
+      <c r="BU24" s="71"/>
+      <c r="BV24" s="71"/>
+      <c r="BW24" s="71"/>
+      <c r="BX24" s="71"/>
+      <c r="BY24" s="71"/>
+      <c r="BZ24" s="71"/>
     </row>
     <row r="25" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="67" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="27"/>
@@ -7078,15 +7063,15 @@
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[Start]])=0,"",IF(AND(BY$5=$E27,$F27=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="BZ25" s="75" t="str">
+      <c r="BZ25" s="69" t="str">
         <f>IFERROR(IF(LEN(Milestones[[#This Row],[No. Days]])=0,"",IF(AND(BZ$5=$E27,$F27=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:78" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
-      <c r="B26" s="73" t="s">
-        <v>45</v>
+      <c r="B26" s="67" t="s">
+        <v>42</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="24">
@@ -7099,57 +7084,57 @@
         <v>5</v>
       </c>
       <c r="G26" s="20"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="76"/>
-      <c r="P26" s="76"/>
-      <c r="Q26" s="76"/>
-      <c r="R26" s="76"/>
-      <c r="S26" s="76"/>
-      <c r="T26" s="76"/>
-      <c r="U26" s="76"/>
-      <c r="V26" s="76"/>
-      <c r="W26" s="76"/>
-      <c r="X26" s="76"/>
-      <c r="Y26" s="76"/>
-      <c r="Z26" s="76"/>
-      <c r="AA26" s="76"/>
-      <c r="AB26" s="76"/>
-      <c r="AC26" s="76"/>
-      <c r="AD26" s="76"/>
-      <c r="AE26" s="76"/>
-      <c r="AF26" s="76"/>
-      <c r="AG26" s="76"/>
-      <c r="AH26" s="76"/>
-      <c r="AI26" s="76"/>
-      <c r="AJ26" s="76"/>
-      <c r="AK26" s="76"/>
-      <c r="AL26" s="76"/>
-      <c r="AM26" s="76"/>
-      <c r="AN26" s="76"/>
-      <c r="AO26" s="76"/>
-      <c r="AP26" s="76"/>
-      <c r="AQ26" s="76"/>
-      <c r="AR26" s="76"/>
-      <c r="AS26" s="76"/>
-      <c r="AT26" s="76"/>
-      <c r="AU26" s="76"/>
-      <c r="AV26" s="76"/>
-      <c r="AW26" s="76"/>
-      <c r="AX26" s="76"/>
-      <c r="AY26" s="76"/>
-      <c r="AZ26" s="76"/>
-      <c r="BA26" s="76"/>
-      <c r="BB26" s="76"/>
-      <c r="BC26" s="76"/>
-      <c r="BD26" s="76"/>
-      <c r="BE26" s="76"/>
-      <c r="BF26" s="82"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="70"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="70"/>
+      <c r="Q26" s="70"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="70"/>
+      <c r="V26" s="70"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="70"/>
+      <c r="Y26" s="70"/>
+      <c r="Z26" s="70"/>
+      <c r="AA26" s="70"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="70"/>
+      <c r="AD26" s="70"/>
+      <c r="AE26" s="70"/>
+      <c r="AF26" s="70"/>
+      <c r="AG26" s="70"/>
+      <c r="AH26" s="70"/>
+      <c r="AI26" s="70"/>
+      <c r="AJ26" s="70"/>
+      <c r="AK26" s="70"/>
+      <c r="AL26" s="70"/>
+      <c r="AM26" s="70"/>
+      <c r="AN26" s="70"/>
+      <c r="AO26" s="70"/>
+      <c r="AP26" s="70"/>
+      <c r="AQ26" s="70"/>
+      <c r="AR26" s="70"/>
+      <c r="AS26" s="70"/>
+      <c r="AT26" s="70"/>
+      <c r="AU26" s="70"/>
+      <c r="AV26" s="70"/>
+      <c r="AW26" s="70"/>
+      <c r="AX26" s="70"/>
+      <c r="AY26" s="70"/>
+      <c r="AZ26" s="70"/>
+      <c r="BA26" s="70"/>
+      <c r="BB26" s="70"/>
+      <c r="BC26" s="70"/>
+      <c r="BD26" s="70"/>
+      <c r="BE26" s="70"/>
+      <c r="BF26" s="76"/>
       <c r="BG26" s="19"/>
       <c r="BH26" s="56"/>
       <c r="BI26" s="56"/>
@@ -7161,102 +7146,102 @@
       <c r="BO26" s="56"/>
       <c r="BP26" s="56"/>
       <c r="BQ26" s="56"/>
-      <c r="BR26" s="82"/>
-      <c r="BS26" s="82"/>
-      <c r="BT26" s="82"/>
-      <c r="BU26" s="82"/>
-      <c r="BV26" s="82"/>
-      <c r="BW26" s="82"/>
-      <c r="BX26" s="82"/>
-      <c r="BY26" s="82"/>
-      <c r="BZ26" s="82"/>
+      <c r="BR26" s="76"/>
+      <c r="BS26" s="76"/>
+      <c r="BT26" s="76"/>
+      <c r="BU26" s="76"/>
+      <c r="BV26" s="76"/>
+      <c r="BW26" s="76"/>
+      <c r="BX26" s="76"/>
+      <c r="BY26" s="76"/>
+      <c r="BZ26" s="76"/>
     </row>
     <row r="27" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="80" t="s">
-        <v>47</v>
+      <c r="B27" s="74" t="s">
+        <v>51</v>
       </c>
       <c r="C27" s="58"/>
       <c r="D27" s="59"/>
       <c r="E27" s="60"/>
       <c r="F27" s="61"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="76"/>
-      <c r="N27" s="76"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
-      <c r="S27" s="76"/>
-      <c r="T27" s="76"/>
-      <c r="U27" s="76"/>
-      <c r="V27" s="76"/>
-      <c r="W27" s="76"/>
-      <c r="X27" s="76"/>
-      <c r="Y27" s="76"/>
-      <c r="Z27" s="76"/>
-      <c r="AA27" s="76"/>
-      <c r="AB27" s="76"/>
-      <c r="AC27" s="76"/>
-      <c r="AD27" s="76"/>
-      <c r="AE27" s="76"/>
-      <c r="AF27" s="76"/>
-      <c r="AG27" s="76"/>
-      <c r="AH27" s="76"/>
-      <c r="AI27" s="76"/>
-      <c r="AJ27" s="76"/>
-      <c r="AK27" s="76"/>
-      <c r="AL27" s="76"/>
-      <c r="AM27" s="76"/>
-      <c r="AN27" s="76"/>
-      <c r="AO27" s="76"/>
-      <c r="AP27" s="76"/>
-      <c r="AQ27" s="76"/>
-      <c r="AR27" s="76"/>
-      <c r="AS27" s="76"/>
-      <c r="AT27" s="76"/>
-      <c r="AU27" s="76"/>
-      <c r="AV27" s="76"/>
-      <c r="AW27" s="76"/>
-      <c r="AX27" s="76"/>
-      <c r="AY27" s="76"/>
-      <c r="AZ27" s="76"/>
-      <c r="BA27" s="76"/>
-      <c r="BB27" s="76"/>
-      <c r="BC27" s="76"/>
-      <c r="BD27" s="76"/>
-      <c r="BE27" s="76"/>
-      <c r="BF27" s="82"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="70"/>
+      <c r="R27" s="70"/>
+      <c r="S27" s="70"/>
+      <c r="T27" s="70"/>
+      <c r="U27" s="70"/>
+      <c r="V27" s="70"/>
+      <c r="W27" s="70"/>
+      <c r="X27" s="70"/>
+      <c r="Y27" s="70"/>
+      <c r="Z27" s="70"/>
+      <c r="AA27" s="70"/>
+      <c r="AB27" s="70"/>
+      <c r="AC27" s="70"/>
+      <c r="AD27" s="70"/>
+      <c r="AE27" s="70"/>
+      <c r="AF27" s="70"/>
+      <c r="AG27" s="70"/>
+      <c r="AH27" s="70"/>
+      <c r="AI27" s="70"/>
+      <c r="AJ27" s="70"/>
+      <c r="AK27" s="70"/>
+      <c r="AL27" s="70"/>
+      <c r="AM27" s="70"/>
+      <c r="AN27" s="70"/>
+      <c r="AO27" s="70"/>
+      <c r="AP27" s="70"/>
+      <c r="AQ27" s="70"/>
+      <c r="AR27" s="70"/>
+      <c r="AS27" s="70"/>
+      <c r="AT27" s="70"/>
+      <c r="AU27" s="70"/>
+      <c r="AV27" s="70"/>
+      <c r="AW27" s="70"/>
+      <c r="AX27" s="70"/>
+      <c r="AY27" s="70"/>
+      <c r="AZ27" s="70"/>
+      <c r="BA27" s="70"/>
+      <c r="BB27" s="70"/>
+      <c r="BC27" s="70"/>
+      <c r="BD27" s="70"/>
+      <c r="BE27" s="70"/>
+      <c r="BF27" s="76"/>
       <c r="BG27" s="19"/>
       <c r="BH27" s="19"/>
       <c r="BI27" s="19"/>
       <c r="BJ27" s="19"/>
-      <c r="BK27" s="82"/>
-      <c r="BL27" s="82"/>
-      <c r="BM27" s="82"/>
-      <c r="BN27" s="82"/>
-      <c r="BO27" s="82"/>
-      <c r="BP27" s="82"/>
-      <c r="BQ27" s="82"/>
-      <c r="BR27" s="82"/>
-      <c r="BS27" s="82"/>
-      <c r="BT27" s="82"/>
-      <c r="BU27" s="82"/>
-      <c r="BV27" s="82"/>
-      <c r="BW27" s="82"/>
-      <c r="BX27" s="82"/>
-      <c r="BY27" s="82"/>
-      <c r="BZ27" s="82"/>
+      <c r="BK27" s="76"/>
+      <c r="BL27" s="76"/>
+      <c r="BM27" s="76"/>
+      <c r="BN27" s="76"/>
+      <c r="BO27" s="76"/>
+      <c r="BP27" s="76"/>
+      <c r="BQ27" s="76"/>
+      <c r="BR27" s="76"/>
+      <c r="BS27" s="76"/>
+      <c r="BT27" s="76"/>
+      <c r="BU27" s="76"/>
+      <c r="BV27" s="76"/>
+      <c r="BW27" s="76"/>
+      <c r="BX27" s="76"/>
+      <c r="BY27" s="76"/>
+      <c r="BZ27" s="76"/>
     </row>
     <row r="28" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="83"/>
+      <c r="B28" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="77"/>
       <c r="D28" s="24">
         <v>0.01</v>
       </c>
@@ -7266,63 +7251,63 @@
       <c r="F28" s="26">
         <v>7</v>
       </c>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="76"/>
-      <c r="S28" s="76"/>
-      <c r="T28" s="76"/>
-      <c r="U28" s="76"/>
-      <c r="V28" s="76"/>
-      <c r="W28" s="76"/>
-      <c r="X28" s="76"/>
-      <c r="Y28" s="76"/>
-      <c r="Z28" s="76"/>
-      <c r="AA28" s="76"/>
-      <c r="AB28" s="76"/>
-      <c r="AC28" s="76"/>
-      <c r="AD28" s="76"/>
-      <c r="AE28" s="76"/>
-      <c r="AF28" s="76"/>
-      <c r="AG28" s="76"/>
-      <c r="AH28" s="76"/>
-      <c r="AI28" s="76"/>
-      <c r="AJ28" s="76"/>
-      <c r="AK28" s="76"/>
-      <c r="AL28" s="76"/>
-      <c r="AM28" s="76"/>
-      <c r="AN28" s="76"/>
-      <c r="AO28" s="76"/>
-      <c r="AP28" s="76"/>
-      <c r="AQ28" s="76"/>
-      <c r="AR28" s="76"/>
-      <c r="AS28" s="76"/>
-      <c r="AT28" s="76"/>
-      <c r="AU28" s="76"/>
-      <c r="AV28" s="76"/>
-      <c r="AW28" s="76"/>
-      <c r="AX28" s="76"/>
-      <c r="AY28" s="76"/>
-      <c r="AZ28" s="76"/>
-      <c r="BA28" s="76"/>
-      <c r="BB28" s="76"/>
-      <c r="BC28" s="76"/>
-      <c r="BD28" s="76"/>
-      <c r="BE28" s="76"/>
-      <c r="BF28" s="82"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="70"/>
+      <c r="Q28" s="70"/>
+      <c r="R28" s="70"/>
+      <c r="S28" s="70"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="70"/>
+      <c r="V28" s="70"/>
+      <c r="W28" s="70"/>
+      <c r="X28" s="70"/>
+      <c r="Y28" s="70"/>
+      <c r="Z28" s="70"/>
+      <c r="AA28" s="70"/>
+      <c r="AB28" s="70"/>
+      <c r="AC28" s="70"/>
+      <c r="AD28" s="70"/>
+      <c r="AE28" s="70"/>
+      <c r="AF28" s="70"/>
+      <c r="AG28" s="70"/>
+      <c r="AH28" s="70"/>
+      <c r="AI28" s="70"/>
+      <c r="AJ28" s="70"/>
+      <c r="AK28" s="70"/>
+      <c r="AL28" s="70"/>
+      <c r="AM28" s="70"/>
+      <c r="AN28" s="70"/>
+      <c r="AO28" s="70"/>
+      <c r="AP28" s="70"/>
+      <c r="AQ28" s="70"/>
+      <c r="AR28" s="70"/>
+      <c r="AS28" s="70"/>
+      <c r="AT28" s="70"/>
+      <c r="AU28" s="70"/>
+      <c r="AV28" s="70"/>
+      <c r="AW28" s="70"/>
+      <c r="AX28" s="70"/>
+      <c r="AY28" s="70"/>
+      <c r="AZ28" s="70"/>
+      <c r="BA28" s="70"/>
+      <c r="BB28" s="70"/>
+      <c r="BC28" s="70"/>
+      <c r="BD28" s="70"/>
+      <c r="BE28" s="70"/>
+      <c r="BF28" s="76"/>
       <c r="BG28" s="19"/>
       <c r="BH28" s="19"/>
       <c r="BI28" s="19"/>
       <c r="BJ28" s="19"/>
-      <c r="BK28" s="82"/>
-      <c r="BL28" s="82"/>
+      <c r="BK28" s="76"/>
+      <c r="BL28" s="76"/>
       <c r="BM28" s="56"/>
       <c r="BN28" s="56"/>
       <c r="BO28" s="56"/>
@@ -7344,77 +7329,77 @@
       </c>
       <c r="C29" s="5"/>
       <c r="F29" s="14"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="76"/>
-      <c r="P29" s="76"/>
-      <c r="Q29" s="76"/>
-      <c r="R29" s="76"/>
-      <c r="S29" s="76"/>
-      <c r="T29" s="76"/>
-      <c r="U29" s="76"/>
-      <c r="V29" s="76"/>
-      <c r="W29" s="76"/>
-      <c r="X29" s="76"/>
-      <c r="Y29" s="76"/>
-      <c r="Z29" s="76"/>
-      <c r="AA29" s="76"/>
-      <c r="AB29" s="76"/>
-      <c r="AC29" s="76"/>
-      <c r="AD29" s="76"/>
-      <c r="AE29" s="76"/>
-      <c r="AF29" s="76"/>
-      <c r="AG29" s="76"/>
-      <c r="AH29" s="76"/>
-      <c r="AI29" s="76"/>
-      <c r="AJ29" s="76"/>
-      <c r="AK29" s="76"/>
-      <c r="AL29" s="76"/>
-      <c r="AM29" s="76"/>
-      <c r="AN29" s="76"/>
-      <c r="AO29" s="76"/>
-      <c r="AP29" s="76"/>
-      <c r="AQ29" s="76"/>
-      <c r="AR29" s="76"/>
-      <c r="AS29" s="76"/>
-      <c r="AT29" s="76"/>
-      <c r="AU29" s="76"/>
-      <c r="AV29" s="76"/>
-      <c r="AW29" s="76"/>
-      <c r="AX29" s="76"/>
-      <c r="AY29" s="76"/>
-      <c r="AZ29" s="76"/>
-      <c r="BA29" s="76"/>
-      <c r="BB29" s="76"/>
-      <c r="BC29" s="76"/>
-      <c r="BD29" s="76"/>
-      <c r="BE29" s="76"/>
-      <c r="BF29" s="82"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="70"/>
+      <c r="P29" s="70"/>
+      <c r="Q29" s="70"/>
+      <c r="R29" s="70"/>
+      <c r="S29" s="70"/>
+      <c r="T29" s="70"/>
+      <c r="U29" s="70"/>
+      <c r="V29" s="70"/>
+      <c r="W29" s="70"/>
+      <c r="X29" s="70"/>
+      <c r="Y29" s="70"/>
+      <c r="Z29" s="70"/>
+      <c r="AA29" s="70"/>
+      <c r="AB29" s="70"/>
+      <c r="AC29" s="70"/>
+      <c r="AD29" s="70"/>
+      <c r="AE29" s="70"/>
+      <c r="AF29" s="70"/>
+      <c r="AG29" s="70"/>
+      <c r="AH29" s="70"/>
+      <c r="AI29" s="70"/>
+      <c r="AJ29" s="70"/>
+      <c r="AK29" s="70"/>
+      <c r="AL29" s="70"/>
+      <c r="AM29" s="70"/>
+      <c r="AN29" s="70"/>
+      <c r="AO29" s="70"/>
+      <c r="AP29" s="70"/>
+      <c r="AQ29" s="70"/>
+      <c r="AR29" s="70"/>
+      <c r="AS29" s="70"/>
+      <c r="AT29" s="70"/>
+      <c r="AU29" s="70"/>
+      <c r="AV29" s="70"/>
+      <c r="AW29" s="70"/>
+      <c r="AX29" s="70"/>
+      <c r="AY29" s="70"/>
+      <c r="AZ29" s="70"/>
+      <c r="BA29" s="70"/>
+      <c r="BB29" s="70"/>
+      <c r="BC29" s="70"/>
+      <c r="BD29" s="70"/>
+      <c r="BE29" s="70"/>
+      <c r="BF29" s="76"/>
       <c r="BG29" s="19"/>
       <c r="BH29" s="19"/>
       <c r="BI29" s="19"/>
       <c r="BJ29" s="19"/>
-      <c r="BK29" s="82"/>
-      <c r="BL29" s="82"/>
-      <c r="BM29" s="82"/>
-      <c r="BN29" s="82"/>
-      <c r="BO29" s="82"/>
-      <c r="BP29" s="82"/>
-      <c r="BQ29" s="82"/>
-      <c r="BR29" s="82"/>
-      <c r="BS29" s="82"/>
-      <c r="BT29" s="82"/>
-      <c r="BU29" s="82"/>
-      <c r="BV29" s="82"/>
-      <c r="BW29" s="82"/>
-      <c r="BX29" s="82"/>
-      <c r="BY29" s="82"/>
-      <c r="BZ29" s="82"/>
+      <c r="BK29" s="76"/>
+      <c r="BL29" s="76"/>
+      <c r="BM29" s="76"/>
+      <c r="BN29" s="76"/>
+      <c r="BO29" s="76"/>
+      <c r="BP29" s="76"/>
+      <c r="BQ29" s="76"/>
+      <c r="BR29" s="76"/>
+      <c r="BS29" s="76"/>
+      <c r="BT29" s="76"/>
+      <c r="BU29" s="76"/>
+      <c r="BV29" s="76"/>
+      <c r="BW29" s="76"/>
+      <c r="BX29" s="76"/>
+      <c r="BY29" s="76"/>
+      <c r="BZ29" s="76"/>
     </row>
     <row r="30" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="6"/>
@@ -7441,37 +7426,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10 H12 N12 H13:M13 R13:U13 L11:N11 M10:P10 S10:Y10 T12:U12 Y12:AE12 W13:X13 AA13:AB13 H14:AC14 AH17:AI17 AN17:AP17 H17:AF18 AH18:AL18 AO18:AP18 AV17:BH17 AV18:AW18 H22:AL22 H21:AM21 AO21:AP21 H19:AX19 H20:AQ20 BC19:BD19 H23:AJ23 AY23:BD23 BG23:BH23 AL23:AW23 AY18:BJ18 AN22:BJ22 AT20:BJ21 BF19:BJ19 H15:AB15 AG15:AW15 BJ23 H25:BF29 H8:BZ8 AD13:BZ13 P11:BZ11 AH12:BZ12 AA10:BZ10 AG14:BZ14 H16:BZ16 BJ17:BZ17 BE15:BZ15 BK18:BZ23 BJ25:BZ25 BR26:BZ26 BK27:BZ27 BK29:BZ29 BK28:BL28">
-    <cfRule type="expression" dxfId="7" priority="87">
+    <cfRule type="expression" dxfId="8" priority="87">
       <formula>H$5&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:BZ5">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>H$5&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:BZ6">
-    <cfRule type="expression" dxfId="5" priority="90">
+    <cfRule type="expression" dxfId="6" priority="90">
       <formula>H$5&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:BK8 K10 H12 N12 H13:M13 R13:U13 L11:N11 M10:P10 S10:Y10 T12:U12 Y12:AE12 P11:BJ11 W13:X13 AA13:AB13 AD13:BJ13 AH12:BJ12 AA10:BJ10 H16:BJ16 AH17:AI17 AN17:AP17 H17:AF18 AH18:AL18 AO18:AP18 AV17:BH17 AV18:AW18 AY18:BJ18 H22:AL22 AN22:BJ22 H21:AM21 AO21:AP21 H19:AX19 H20:AQ20 AT20:BJ21 BC19:BD19 BF19:BJ19 H23:AJ23 AY23:BD23 BG23:BH23 AL23:AW23 BJ17 BJ23 BJ25 H25:BF25 BL8:BZ8">
-    <cfRule type="expression" dxfId="4" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="91" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E7+1,H$5&lt;=$E7+$F7-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:AC14 AG14:BJ14 H15:AB15 AG15:AW15 BE15:BJ15 BK13:BZ13">
-    <cfRule type="expression" dxfId="3" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="94" stopIfTrue="1">
       <formula>AND(H$5&gt;=#REF!+1,H$5&lt;=#REF!+#REF!-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK10:BZ12 BK16:BZ22 BR26:BZ26 BK27:BZ27 BK29:BZ29 BK28:BL28">
-    <cfRule type="expression" dxfId="2" priority="109" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="109" stopIfTrue="1">
       <formula>AND(BK$5&gt;=$E11+1,BK$5&lt;=$E11+$F11-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK14:BZ15 BK23:BZ23 BK25:BZ25">
-    <cfRule type="expression" dxfId="1" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="154" stopIfTrue="1">
       <formula>AND(BK$5&gt;=$E16+1,BK$5&lt;=$E16+$F16-2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7504,7 +7489,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:BF29">
-    <cfRule type="expression" dxfId="0" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="158" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E25+1,H$5&lt;=$E25+$F25-2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7574,25 +7559,6 @@
           <xm:sqref>D6:D26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="11" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
-            <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Signs" iconId="1"/>
-              <x14:cfIcon iconSet="3Flags" iconId="0"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>F4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4EE6D036-95FE-4F7E-B435-81BDF75365C6}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -7621,6 +7587,25 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>D28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="11" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
+            <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="160" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">

</xml_diff>